<commit_message>
Added the SRS_ID related to the test case
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TESTCASES.xlsx
+++ b/LH_TESTCASES/LH_TESTCASES.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>TC_ID</t>
   </si>
@@ -46,24 +46,6 @@
   </si>
   <si>
     <t>Severity</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
-    <t>TC006</t>
   </si>
   <si>
     <t>LH-TC-Login-001</t>
@@ -277,13 +259,28 @@
   </si>
   <si>
     <t>modify after last reviewers comments on version 1.1 of TC</t>
+  </si>
+  <si>
+    <t>SRS-LOGIN-001</t>
+  </si>
+  <si>
+    <t>SRS-LOGIN-003</t>
+  </si>
+  <si>
+    <t>SRS-LOGIN-002</t>
+  </si>
+  <si>
+    <t>Added the SRS_ID related to the test case</t>
+  </si>
+  <si>
+    <t>v1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,13 +313,6 @@
     </font>
     <font>
       <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -395,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,20 +421,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1056,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="44" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScale="44" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25"/>
@@ -1082,25 +1071,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -1116,259 +1105,259 @@
     </row>
     <row r="2" spans="1:13" ht="85.5">
       <c r="A2" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="I2" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="85.5">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="85.5">
       <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="85.5">
       <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="85.5">
       <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>38</v>
+        <v>68</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="85.5">
       <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="J7" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" ht="85.5">
       <c r="A8" s="9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1440,7 +1429,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1452,52 +1441,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>58</v>
+      <c r="A1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="18">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="17">
         <v>45760</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="56.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="17">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="18">
+      <c r="B4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="17">
         <v>45766</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>